<commit_message>
a1:merge issue resolved with Keras final notebook
</commit_message>
<xml_diff>
--- a/Citations.xlsx
+++ b/Citations.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988E2C58-2102-4DDA-8AF7-DE0E86377205}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F688E7-7BA8-4EFF-BC37-4C6046AF4678}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21390" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21390" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SLP" sheetId="4" r:id="rId1"/>
     <sheet name="CNN" sheetId="1" r:id="rId2"/>
     <sheet name="Links" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CNN!$D$1:$D$11</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="242">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -1399,12 +1400,563 @@
   <si>
     <t>https://github.com/BayesWatch/cinic-10</t>
   </si>
+  <si>
+    <t>Weiss, K, Khoshgoftaar, TM &amp; Wang, D 2016, ‘A survey of transfer learning’, Journal of Big Data, vol. 3, no. 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#@article{WeissKarl2016Asot,
+abstract = {Machine learning and data mining techniques have been used in numerous real-world applications. An assumption of traditional machine learning methodologies is the training data and testing data are taken from the same domain, such that the input feature space and data distribution characteristics are the same. However, in some real-world machine learning scenarios, this assumption does not hold. There are cases where training data is expensive or difficult to collect. Therefore, there is a need to create high-performance learners trained with more easily obtained data from different domains. This methodology is referred to as transfer learning. This survey paper formally defines transfer learning, presents information on current solutions, and reviews applications applied to transfer learning. Lastly, there is information listed on software downloads for various transfer learning solutions and a discussion of possible future research work. The transfer learning solutions surveyed are independent of data size and can be applied to big data environments.},
+author = {Weiss, Karl and Khoshgoftaar, Taghi M. and Wang, DingDing},
+address = {Cham},
+copyright = {The Author(s) 2016},
+issn = {2196-1115},
+journal = {Journal of big data},
+keywords = {Communications Engineering ; Computational Science and Engineering ; Computer Science ; Data mining ; Data Mining and Knowledge Discovery ; Database Management ; Domain adaptation ; Information Storage and Retrieval ; Machine learning ; Mathematical Applications in Computer Science ; Networks ; Survey ; Survey Paper ; Transfer learning},
+language = {eng},
+number = {1},
+publisher = {Springer International Publishing},
+title = {A survey of transfer learning},
+volume = {3},
+year = {2016},
+}
+</t>
+  </si>
+  <si>
+    <t>Tan, C, Sun, F, Kong, T, Zhang, W, Yang, C &amp; Liu, C 2018, ‘A Survey on Deep Transfer Learning’, in Artificial Neural Networks and Machine Learning – ICANN 2018, vol. 11141, Springer International Publishing, Cham, pp. 270–279.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#@incollection{TanChuanqi2018ASoD,
+abstract = {As a new classification platform, deep learning has recently received increasing attention from researchers and has been successfully applied to many domains. In some domains, like bioinformatics and robotics, it is very difficult to construct a large-scale well-annotated dataset due to the expense of data acquisition and costly annotation, which limits its development. Transfer learning relaxes the hypothesis that the training data must be independent and identically distributed (i.i.d.) with the test data, which motivates us to use transfer learning to solve the problem of insufficient training data. This survey focuses on reviewing the current researches of transfer learning by using deep neural network and its applications. We defined deep transfer learning, category and review the recent research works based on the techniques used in deep transfer learning.},
+author = {Tan, Chuanqi and Sun, Fuchun and Kong, Tao and Zhang, Wenchang and Yang, Chao and Liu, Chunfang},
+address = {Cham},
+booktitle = {Artificial Neural Networks and Machine Learning – ICANN 2018},
+copyright = {Springer Nature Switzerland AG 2018},
+isbn = {9783030014230},
+issn = {0302-9743},
+keywords = {Deep transfer learning ; Survey ; Transfer learning},
+language = {eng},
+pages = {270-279},
+publisher = {Springer International Publishing},
+series = {Lecture Notes in Computer Science},
+title = {A Survey on Deep Transfer Learning},
+volume = {11141},
+year = {2018},
+}
+</t>
+  </si>
+  <si>
+    <t>Transfer Learning</t>
+  </si>
+  <si>
+    <t>Yosinski, J, Clune, J, Bengio, Y &amp; Lipson, H 2014, ‘How transferable are features in deep neural networks?’, arXiv.org.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#@article{YosinskiJason2014Htaf,
+abstract = {Many deep neural networks trained on natural images exhibit a curious phenomenon in common: on the first layer they learn features similar to Gabor filters and color blobs. Such first-layer features appear not to be specific to a particular dataset or task, but general in that they are applicable to many datasets and tasks. Features must eventually transition from general to specific by the last layer of the network, but this transition has not been studied extensively. In this paper we experimentally quantify the generality versus specificity of neurons in each layer of a deep convolutional neural network and report a few surprising results. Transferability is negatively affected by two distinct issues: (1) the specialization of higher layer neurons to their original task at the expense of performance on the target task, which was expected, and (2) optimization difficulties related to splitting networks between co-adapted neurons, which was not expected. In an example network trained on ImageNet, we demonstrate that either of these two issues may dominate, depending on whether features are transferred from the bottom, middle, or top of the network. We also document that the transferability of features decreases as the distance between the base task and target task increases, but that transferring features even from distant tasks can be better than using random features. A final surprising result is that initializing a network with transferred features from almost any number of layers can produce a boost to generalization that lingers even after fine-tuning to the target dataset.},
+author = {Yosinski, Jason and Clune, Jeff and Bengio, Yoshua and Lipson, Hod},
+address = {Ithaca},
+copyright = {2014. This work is published under http://arxiv.org/licenses/nonexclusive-distrib/1.0/ (the “License”). Notwithstanding the ProQuest Terms and Conditions, you may use this content in accordance with the terms of the License.},
+issn = {2331-8422},
+journal = {arXiv.org},
+keywords = {Artificial neural networks ; Gabor filters ; Neural networks ; Neurons ; Optimization},
+language = {eng},
+publisher = {Cornell University Library, arXiv.org},
+title = {How transferable are features in deep neural networks?},
+year = {2014},
+}
+</t>
+  </si>
+  <si>
+    <t>Long, M, Zhu, H, Wang, J &amp; Jordan, MI 2017, ‘Unsupervised Domain Adaptation with Residual Transfer Networks’, arXiv.org.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#@article{LongMingsheng2017UDAw,
+abstract = {The recent success of deep neural networks relies on massive amounts of labeled data. For a target task where labeled data is unavailable, domain adaptation can transfer a learner from a different source domain. In this paper, we propose a new approach to domain adaptation in deep networks that can jointly learn adaptive classifiers and transferable features from labeled data in the source domain and unlabeled data in the target domain. We relax a shared-classifier assumption made by previous methods and assume that the source classifier and target classifier differ by a residual function. We enable classifier adaptation by plugging several layers into deep network to explicitly learn the residual function with reference to the target classifier. We fuse features of multiple layers with tensor product and embed them into reproducing kernel Hilbert spaces to match distributions for feature adaptation. The adaptation can be achieved in most feed-forward models by extending them with new residual layers and loss functions, which can be trained efficiently via back-propagation. Empirical evidence shows that the new approach outperforms state of the art methods on standard domain adaptation benchmarks.},
+author = {Long, Mingsheng and Zhu, Han and Wang, Jianmin and Jordan, Michael I},
+address = {Ithaca},
+copyright = {2017. This work is published under http://arxiv.org/licenses/nonexclusive-distrib/1.0/ (the “License”). Notwithstanding the ProQuest Terms and Conditions, you may use this content in accordance with the terms of the License.},
+issn = {2331-8422},
+journal = {arXiv.org},
+keywords = {Adaptation ; Back propagation ; Classifiers ; Computer Science - Learning ; Hilbert space ; Neural networks ; Tensors},
+language = {eng},
+publisher = {Cornell University Library, arXiv.org},
+title = {Unsupervised Domain Adaptation with Residual Transfer Networks},
+year = {2017},
+}
+</t>
+  </si>
+  <si>
+    <t>Pan, SJ &amp; Yang, Q 2010, ‘A Survey on Transfer Learning’, IEEE Transactions on Knowledge and Data Engineering, vol. 22, no. 10, pp. 1345–1359.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#@article{PanSinnoJialin2010ASoT,
+abstract = {A major assumption in many machine learning and data mining algorithms is that the training and future data must be in the same feature space and have the same distribution. However, in many real-world applications, this assumption may not hold. For example, we sometimes have a classification task in one domain of interest, but we only have sufficient training data in another domain of interest, where the latter data may be in a different feature space or follow a different data distribution. In such cases, knowledge transfer, if done successfully, would greatly improve the performance of learning by avoiding much expensive data-labeling efforts. In recent years, transfer learning has emerged as a new learning framework to address this problem. This survey focuses on categorizing and reviewing the current progress on transfer learning for classification, regression, and clustering problems. In this survey, we discuss the relationship between transfer learning and other related machine learning techniques such as domain adaptation, multitask learning and sample selection bias, as well as covariate shift. We also explore some potential future issues in transfer learning research.},
+author = {Pan, Sinno Jialin and Yang, Qiang},
+address = {LOS ALAMITOS},
+copyright = {Copyright 2010 Elsevier B.V., All rights reserved.},
+issn = {1041-4347},
+journal = {IEEE transactions on knowledge and data engineering},
+keywords = {Adaptation ; Algorithms ; Applied sciences ; Artificial intelligence ; Classification ; Computer Science ; Computer Science, Artificial Intelligence ; Computer Science, Information Systems ; Computer science; control theory; systems ; Data mining ; Data processing. List processing. Character string processing ; Engineering ; Engineering, Electrical &amp; Electronic ; Exact sciences and technology ; Information systems. Data bases ; Knowledge engineering ; Knowledge transfer ; Labeling ; Learning ; Learning systems ; Machine learning ; Machine learning algorithms ; Memory organisation. Data processing ; Regression ; Science &amp; Technology ; Software ; Space technology ; Studies ; survey ; Tasks ; Technology ; Testing ; Training ; Training data ; Transfer learning},
+language = {eng},
+number = {10},
+pages = {1345-1359},
+publisher = {IEEE},
+title = {A Survey on Transfer Learning},
+volume = {22},
+year = {2010},
+}
+</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>AlexNet</t>
+  </si>
+  <si>
+    <t>Fukushima, K., 1980. Neocognitron: A self-organizing neural network model for a mechanism of pattern recognition unaffected by shift in position. Biological cybernetics, 36(4), pp.193-202.</t>
+  </si>
+  <si>
+    <t>#@article{fukushima1980neocognitron,
+  title={Neocognitron: A self-organizing neural network model for a mechanism of pattern recognition unaffected by shift in position},
+  author={Fukushima, Kunihiko},
+  journal={Biological cybernetics},
+  volume={36},
+  number={4},
+  pages={193--202},
+  year={1980},
+  publisher={Springer}
+}</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>cnn 1st
+OG</t>
+  </si>
+  <si>
+    <t>Hubel, D.H. and Wiesel, T.N., 1968. Receptive fields and functional architecture of monkey striate cortex. The Journal of physiology, 195(1), pp.215-243.</t>
+  </si>
+  <si>
+    <t>#@article{hubel1968receptive,
+  title={Receptive fields and functional architecture of monkey striate cortex},
+  author={Hubel, David H and Wiesel, Torsten N},
+  journal={The Journal of physiology},
+  volume={195},
+  number={1},
+  pages={215--243},
+  year={1968},
+  publisher={Wiley Online Library}
+}</t>
+  </si>
+  <si>
+    <t>Waibel, A, Hanazawa, T, Hinton, G, Shikano, K &amp; Lang, KJ 1989, ‘Phoneme recognition using time-delay neural networks’, IEEE Transactions on Acoustics, Speech, and Signal Processing, vol. 37, no. 3, pp. 328–339.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#@article{WaibelA.1989Prut,
+abstract = {The authors present a time-delay neural network (TDNN) approach to phoneme recognition which is characterized by two important properties: (1) using a three-layer arrangement of simple computing units, a hierarchy can be constructed that allows for the formation of arbitrary nonlinear decision surfaces, which the TDNN learns automatically using error backpropagation; and (2) the time-delay arrangement enables the network to discover acoustic-phonetic features and the temporal relationships between them independently of position in time and therefore not blurred by temporal shifts in the input. As a recognition task, the speaker-dependent recognition of the phonemes B, D, and G in varying phonetic contexts was chosen. For comparison, several discrete hidden Markov models (HMM) were trained to perform the same task. Performance evaluation over 1946 testing tokens from three speakers showed that the TDNN achieves a recognition rate of 98.5% correct while the rate obtained by the best of the HMMs was only 93.7%.&lt; &gt;},
+author = {Waibel, A. and Hanazawa, T. and Hinton, G. and Shikano, K. and Lang, K.J.},
+address = {NEW YORK},
+copyright = {Copyright 2015 Elsevier B.V., All rights reserved.},
+issn = {0096-3518},
+journal = {IEEE transactions on acoustics, speech, and signal processing},
+keywords = {Acoustic testing ; Acoustics ; Backpropagation ; Character recognition ; Computer networks ; Computer science ; Engineering ; Engineering, Electrical &amp; Electronic ; Hidden Markov models ; Loudspeakers ; Neural networks ; Psychology ; Science &amp; Technology ; Speech recognition ; Technology},
+language = {eng},
+number = {3},
+pages = {328-339},
+publisher = {IEEE},
+title = {Phoneme recognition using time-delay neural networks},
+volume = {37},
+year = {1989},
+}
+</t>
+  </si>
+  <si>
+    <t>Yamaguchi, K., Sakamoto, K., Akabane, T. and Fujimoto, Y., 1990, November. A neural network for speaker-independent isolated word recognition. In ICSLP.</t>
+  </si>
+  <si>
+    <t>#@inproceedings{yamaguchi1990neural,
+  title={A neural network for speaker-independent isolated word recognition.},
+  author={Yamaguchi, Kouichi and Sakamoto, Kenji and Akabane, Toshio and Fujimoto, Yoshiji},
+  booktitle={ICSLP},
+  year={1990}
+}</t>
+  </si>
+  <si>
+    <t>CNN History</t>
+  </si>
+  <si>
+    <t>shift invariance
+backpropogation</t>
+  </si>
+  <si>
+    <t>biological processes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max pooling </t>
+  </si>
+  <si>
+    <t>LeCun, Y., Bottou, L., Bengio, Y. and Haffner, P., 1998. Gradient-based learning applied to document recognition. Proceedings of the IEEE, 86(11), pp.2278-2324.</t>
+  </si>
+  <si>
+    <t>#@article{lecun1989backpropagation,
+  title={Backpropagation applied to handwritten zip code recognition},
+  author={LeCun, Yann and Boser, Bernhard and Denker, John S and Henderson, Donnie and Howard, Richard E and Hubbard, Wayne and Jackel, Lawrence D},
+  journal={Neural computation},
+  volume={1},
+  number={4},
+  pages={541--551},
+  year={1989},
+  publisher={MIT Press}
+}</t>
+  </si>
+  <si>
+    <t>Gradient Descent</t>
+  </si>
+  <si>
+    <t>#@article{russakovsky2015imagenet,
+  title={Imagenet large scale visual recognition challenge},
+  author={Russakovsky, Olga and Deng, Jia and Su, Hao and Krause, Jonathan and Satheesh, Sanjeev and Ma, Sean and Huang, Zhiheng and Karpathy, Andrej and Khosla, Aditya and Bernstein, Michael and others},
+  journal={International journal of computer vision},
+  volume={115},
+  pages={211--252},
+  year={2015},
+  publisher={Springer}
+}</t>
+  </si>
+  <si>
+    <r>
+      <t>Russakovsky, O., Deng, J., Su, H., Krause, J., Satheesh, S., Ma, S., Huang, Z., Karpathy, A., Khosla, A., Bernstein, M. and Berg, A.C., 2015. Imagenet large scale visual recognition challenge. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>International journal of computer vision</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>115</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, pp.211-252.</t>
+    </r>
+  </si>
+  <si>
+    <t>West, J., Ventura, D. and Warnick, S., 2007. Spring research presentation: A theoretical foundation for inductive transfer. Brigham Young University, College of Physical and Mathematical Sciences, 1(08).</t>
+  </si>
+  <si>
+    <t>#@article{west2007spring,
+  title={Spring research presentation: A theoretical foundation for inductive transfer},
+  author={West, Jeremy and Ventura, Dan and Warnick, Sean},
+  journal={Brigham Young University, College of Physical and Mathematical Sciences},
+  volume={1},
+  number={08},
+  year={2007}
+}</t>
+  </si>
+  <si>
+    <t>Basic Definition</t>
+  </si>
+  <si>
+    <t>Zeiler, M.D. and Fergus, R., 2014. Visualizing and understanding convolutional networks. In Computer Vision–ECCV 2014: 13th European Conference, Zurich, Switzerland, September 6-12, 2014, Proceedings, Part I 13 (pp. 818-833). Springer International Publishing.</t>
+  </si>
+  <si>
+    <t>#@inproceedings{zeiler2014visualizing,
+  title={Visualizing and understanding convolutional networks},
+  author={Zeiler, Matthew D and Fergus, Rob},
+  booktitle={Computer Vision--ECCV 2014: 13th European Conference, Zurich, Switzerland, September 6-12, 2014, Proceedings, Part I 13},
+  pages={818--833},
+  year={2014},
+  organization={Springer}
+}</t>
+  </si>
+  <si>
+    <t>ZFNet</t>
+  </si>
+  <si>
+    <t>Simonyan, K. and Zisserman, A., 2014. Very deep convolutional networks for large-scale image recognition. arXiv preprint arXiv:1409.1556.</t>
+  </si>
+  <si>
+    <t>#@article{simonyan2014very,
+  title={Very deep convolutional networks for large-scale image recognition},
+  author={Simonyan, Karen and Zisserman, Andrew},
+  journal={arXiv preprint arXiv:1409.1556},
+  year={2014}
+}</t>
+  </si>
+  <si>
+    <t>VGG</t>
+  </si>
+  <si>
+    <t>He, K., Zhang, X., Ren, S. and Sun, J., 2016. Deep residual learning for image recognition. In Proceedings of the IEEE conference on computer vision and pattern recognition (pp. 770-778).</t>
+  </si>
+  <si>
+    <t>#@inproceedings{he2016deep,
+  title={Deep residual learning for image recognition},
+  author={He, Kaiming and Zhang, Xiangyu and Ren, Shaoqing and Sun, Jian},
+  booktitle={Proceedings of the IEEE conference on computer vision and pattern recognition},
+  pages={770--778},
+  year={2016}
+}</t>
+  </si>
+  <si>
+    <t>Szegedy, C., Liu, W., Jia, Y., Sermanet, P., Reed, S., Anguelov, D., Erhan, D., Vanhoucke, V. and Rabinovich, A., 2015. Going deeper with convolutions. In Proceedings of the IEEE conference on computer vision and pattern recognition (pp. 1-9).</t>
+  </si>
+  <si>
+    <t>#@inproceedings{szegedy2015going,
+  title={Going deeper with convolutions},
+  author={Szegedy, Christian and Liu, Wei and Jia, Yangqing and Sermanet, Pierre and Reed, Scott and Anguelov, Dragomir and Erhan, Dumitru and Vanhoucke, Vincent and Rabinovich, Andrew},
+  booktitle={Proceedings of the IEEE conference on computer vision and pattern recognition},
+  pages={1--9},
+  year={2015}
+}</t>
+  </si>
+  <si>
+    <t>GoogleNet</t>
+  </si>
+  <si>
+    <t>Resnet</t>
+  </si>
+  <si>
+    <t>Model name</t>
+  </si>
+  <si>
+    <r>
+      <t>Number of parameters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF2F4858"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> [Millions]</t>
+    </r>
+  </si>
+  <si>
+    <t>ImageNet Top 1 Accuracy</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>60 M</t>
+  </si>
+  <si>
+    <t>Inception V1</t>
+  </si>
+  <si>
+    <t>5 M</t>
+  </si>
+  <si>
+    <t>VGG 16</t>
+  </si>
+  <si>
+    <t>138 M</t>
+  </si>
+  <si>
+    <t>ResNet-50</t>
+  </si>
+  <si>
+    <t>26 M</t>
+  </si>
+  <si>
+    <t>Network Based</t>
+  </si>
+  <si>
+    <t>Krizhevsky, A. and Hinton, G., 2009. Learning multiple layers of features from tiny images.</t>
+  </si>
+  <si>
+    <t>#@article{krizhevsky2009learning,
+  title={Learning multiple layers of features from tiny images},
+  author={Krizhevsky, Alex and Hinton, Geoffrey and others},
+  year={2009},
+  publisher={Toronto, ON, Canada}
+}</t>
+  </si>
+  <si>
+    <t>CIFAR-10</t>
+  </si>
+  <si>
+    <t>Deng, J., Dong, W., Socher, R., Li, L.J., Li, K. and Fei-Fei, L., 2009, June. Imagenet: A large-scale hierarchical image database. In 2009 IEEE conference on computer vision and pattern recognition (pp. 248-255). Ieee.</t>
+  </si>
+  <si>
+    <t>#@inproceedings{deng2009imagenet,
+  title={Imagenet: A large-scale hierarchical image database},
+  author={Deng, Jia and Dong, Wei and Socher, Richard and Li, Li-Jia and Li, Kai and Fei-Fei, Li},
+  booktitle={2009 IEEE conference on computer vision and pattern recognition},
+  pages={248--255},
+  year={2009},
+  organization={Ieee}
+}</t>
+  </si>
+  <si>
+    <t>Chrabaszcz, P., Loshchilov, I. and Hutter, F., 2017. A downsampled variant of imagenet as an alternative to the cifar datasets. arXiv preprint arXiv:1707.08819.</t>
+  </si>
+  <si>
+    <t>#@article{chrabaszcz2017downsampled,
+  title={A downsampled variant of imagenet as an alternative to the cifar datasets},
+  author={Chrabaszcz, Patryk and Loshchilov, Ilya and Hutter, Frank},
+  journal={arXiv preprint arXiv:1707.08819},
+  year={2017}
+}</t>
+  </si>
+  <si>
+    <t>Nothiing to be quoted</t>
+  </si>
+  <si>
+    <t>Imagenet-64</t>
+  </si>
+  <si>
+    <t>Imagenet</t>
+  </si>
+  <si>
+    <t>Neyshabur, B., Sedghi, H. and Zhang, C., 2020. What is being transferred in transfer learning?. Advances in neural information processing systems, 33, pp.512-523.</t>
+  </si>
+  <si>
+    <t>#@article{neyshabur2020being,
+  title={What is being transferred in transfer learning?},
+  author={Neyshabur, Behnam and Sedghi, Hanie and Zhang, Chiyuan},
+  journal={Advances in neural information processing systems},
+  volume={33},
+  pages={512--523},
+  year={2020}
+}</t>
+  </si>
+  <si>
+    <t>Bau, B. Zhou, A. Khosla, A. Oliva, and A. Torralba. Network dissection: Quantifying interpretability
+of deep visual representations. In Proceedings of the IEEE conference on computer
+vision and pattern recognition, pages 6541–6549, 2017.</t>
+  </si>
+  <si>
+    <t>#@inproceedings{bau2017network,
+  title={Network dissection: Quantifying interpretability of deep visual representations},
+  author={Bau, David and Zhou, Bolei and Khosla, Aditya and Oliva, Aude and Torralba, Antonio},
+  booktitle={Proceedings of the IEEE conference on computer vision and pattern recognition},
+  pages={6541--6549},
+  year={2017}
+}</t>
+  </si>
+  <si>
+    <t>Pardede, J., Sitohang, B., Akbar, S. and Khodra, M.L., 2021. Implementation of transfer learning using VGG16 on fruit ripeness detection. Int. J. Intell. Syst. Appl, 13(2), pp.52-61.</t>
+  </si>
+  <si>
+    <t>#@article{pardede2021implementation,
+  title={Implementation of transfer learning using VGG16 on fruit ripeness detection},
+  author={Pardede, Jasman and Sitohang, Benhard and Akbar, Saiful and Khodra, Masayu Leylia},
+  journal={Int. J. Intell. Syst. Appl},
+  volume={13},
+  number={2},
+  pages={52--61},
+  year={2021}
+}</t>
+  </si>
+  <si>
+    <t>Pannell, J.J., Rigby, S.E. and Panoutsos, G., 2023. Application of transfer learning for the prediction of blast impulse. International Journal of Protective Structures, 14(2), pp.242-262.</t>
+  </si>
+  <si>
+    <t>#@article{pannell2023application,
+  title={Application of transfer learning for the prediction of blast impulse},
+  author={Pannell, Jordan J and Rigby, Sam E and Panoutsos, George},
+  journal={International Journal of Protective Structures},
+  volume={14},
+  number={2},
+  pages={242--262},
+  year={2023},
+  publisher={SAGE Publications Sage UK: London, England}
+}</t>
+  </si>
+  <si>
+    <t>Voulodimos, A., Doulamis, N., Doulamis, A. and Protopapadakis, E., 2018. Deep learning for computer vision: A brief review. Computational intelligence and neuroscience, 2018.</t>
+  </si>
+  <si>
+    <t>#@article{voulodimos2018deep,
+  title={Deep learning for computer vision: A brief review},
+  author={Voulodimos, Athanasios and Doulamis, Nikolaos and Doulamis, Anastasios and Protopapadakis, Eftychios and others},
+  journal={Computational intelligence and neuroscience},
+  volume={2018},
+  year={2018},
+  publisher={Hindawi}
+}</t>
+  </si>
+  <si>
+    <t>Wu, H. and Gu, X., 2015. Max-pooling dropout for regularization of convolutional neural networks. In Neural Information Processing: 22nd International Conference, ICONIP 2015, Istanbul, Turkey, November 9-12, 2015, Proceedings, Part I 22 (pp. 46-54). Springer International Publishing.</t>
+  </si>
+  <si>
+    <t>#@inproceedings{wu2015max,
+  title={Max-pooling dropout for regularization of convolutional neural networks},
+  author={Wu, Haibing and Gu, Xiaodong},
+  booktitle={Neural Information Processing: 22nd International Conference, ICONIP 2015, Istanbul, Turkey, November 9-12, 2015, Proceedings, Part I 22},
+  pages={46--54},
+  year={2015},
+  organization={Springer}
+}</t>
+  </si>
+  <si>
+    <t>He, T., Zhang, Z., Zhang, H., Zhang, Z., Xie, J. and Li, M., 2019. Bag of tricks for image classification with convolutional neural networks. In Proceedings of the IEEE/CVF conference on computer vision and pattern recognition (pp. 558-567).</t>
+  </si>
+  <si>
+    <t>3@inproceedings{he2019bag,
+  title={Bag of tricks for image classification with convolutional neural networks},
+  author={He, Tong and Zhang, Zhi and Zhang, Hang and Zhang, Zhongyue and Xie, Junyuan and Li, Mu},
+  booktitle={Proceedings of the IEEE/CVF conference on computer vision and pattern recognition},
+  pages={558--567},
+  year={2019}
+}</t>
+  </si>
+  <si>
+    <t>Data Augmentation</t>
+  </si>
+  <si>
+    <t>#@misc{Gavrikov2020VisualKeras,
+  author = {Gavrikov, Paul},
+  title = {visualkeras},
+  year = {2020},
+  publisher = {GitHub},
+  journal = {GitHub repository},
+  howpublished = {\url{https://github.com/paulgavrikov/visualkeras}},
+}</t>
+  </si>
+  <si>
+    <t>VISUAL KERAS</t>
+  </si>
+  <si>
+    <t>VisualKeras</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1472,8 +2024,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF2F4858"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF2F4858"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1510,8 +2088,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F8F8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1571,12 +2161,151 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1734,13 +2463,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF2F4858"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1751,6 +2606,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1B67B3AD-5FA4-433C-B28C-8AA06D7EC626}" name="Table1" displayName="Table1" ref="A2:E6" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1" totalsRowBorderDxfId="0">
+  <autoFilter ref="A2:E6" xr:uid="{07394959-5844-4759-A2C5-3CA0214E97C0}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{C1F99881-D5DA-4153-AC06-D3698B3F86FA}" name="Sr. No."/>
+    <tableColumn id="2" xr3:uid="{B44C6772-1D4E-434D-BAFA-3A87232DB6F4}" name="Model name"/>
+    <tableColumn id="3" xr3:uid="{6EE3932E-C13D-40D1-959E-5EA77DBF27E8}" name="Number of parameters [Millions]"/>
+    <tableColumn id="4" xr3:uid="{784E4F9C-4AF5-43B2-838B-4CB8E9423526}" name="ImageNet Top 1 Accuracy"/>
+    <tableColumn id="5" xr3:uid="{9D42CA59-608A-40A3-A6CF-6965FFC5E1AA}" name="Year"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2877,10 +3746,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView topLeftCell="D26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView topLeftCell="A53" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3232,7 +4101,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="48" t="s">
         <v>88</v>
@@ -3288,8 +4157,12 @@
       <c r="G16" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -3469,7 +4342,9 @@
       <c r="G25" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H25" s="3"/>
+      <c r="H25" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3488,7 +4363,9 @@
       <c r="G26" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H26" s="3"/>
+      <c r="H26" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3577,265 +4454,399 @@
         <v>153</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="4"/>
+      <c r="B31" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>155</v>
+      </c>
       <c r="D31" s="33"/>
       <c r="E31" s="33"/>
-      <c r="F31" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G31" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H31" s="3"/>
+      <c r="F31" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="D32" s="33"/>
       <c r="E32" s="33"/>
-      <c r="F32" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G32" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F32" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="4"/>
+      <c r="B33" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>160</v>
+      </c>
       <c r="D33" s="33"/>
       <c r="E33" s="33"/>
-      <c r="F33" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G33" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F33" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="4"/>
+      <c r="B34" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="82" t="s">
+        <v>162</v>
+      </c>
       <c r="D34" s="33"/>
       <c r="E34" s="33"/>
-      <c r="F34" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G34" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H34" s="3"/>
+      <c r="F34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="33"/>
+      <c r="B35" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="C35" s="84" t="s">
+        <v>164</v>
+      </c>
+      <c r="D35" s="81"/>
       <c r="E35" s="33"/>
-      <c r="F35" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G35" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H35" s="3"/>
+      <c r="F35" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="4"/>
+      <c r="B36" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="C36" s="83" t="s">
+        <v>168</v>
+      </c>
       <c r="D36" s="33"/>
       <c r="E36" s="33"/>
-      <c r="F36" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G36" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F36" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="4"/>
+      <c r="B37" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>172</v>
+      </c>
       <c r="D37" s="33"/>
       <c r="E37" s="33"/>
-      <c r="F37" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G37" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="4"/>
+      <c r="B38" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>174</v>
+      </c>
       <c r="D38" s="33"/>
       <c r="E38" s="33"/>
-      <c r="F38" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G38" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="4"/>
+      <c r="B39" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>176</v>
+      </c>
       <c r="D39" s="33"/>
       <c r="E39" s="33"/>
-      <c r="F39" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G39" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="4"/>
+      <c r="B40" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>182</v>
+      </c>
       <c r="D40" s="33"/>
       <c r="E40" s="33"/>
-      <c r="F40" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G40" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F40" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="4"/>
+      <c r="B41" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="C41" s="65" t="s">
+        <v>186</v>
+      </c>
       <c r="D41" s="33"/>
       <c r="E41" s="33"/>
-      <c r="F41" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G41" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F41" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="4"/>
+      <c r="B42" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>187</v>
+      </c>
       <c r="D42" s="33"/>
       <c r="E42" s="33"/>
       <c r="F42" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="G42" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G42" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="4"/>
+      <c r="B43" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>190</v>
+      </c>
       <c r="D43" s="33"/>
       <c r="E43" s="33"/>
-      <c r="F43" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G43" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F43" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
-      <c r="B44" s="48"/>
-      <c r="C44" s="4"/>
+      <c r="B44" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>193</v>
+      </c>
       <c r="D44" s="33"/>
       <c r="E44" s="33"/>
-      <c r="F44" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G44" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F44" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
-      <c r="B45" s="48"/>
-      <c r="C45" s="4"/>
+      <c r="B45" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>196</v>
+      </c>
       <c r="D45" s="33"/>
       <c r="E45" s="33"/>
-      <c r="F45" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G45" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F45" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
-      <c r="B46" s="48"/>
-      <c r="C46" s="4"/>
+      <c r="B46" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>198</v>
+      </c>
       <c r="D46" s="33"/>
       <c r="E46" s="33"/>
-      <c r="F46" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G46" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F46" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="4"/>
+      <c r="B47" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>214</v>
+      </c>
       <c r="D47" s="33"/>
       <c r="E47" s="33"/>
-      <c r="F47" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G47" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F47" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
-      <c r="B48" s="48"/>
-      <c r="C48" s="4"/>
+      <c r="B48" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>217</v>
+      </c>
       <c r="D48" s="33"/>
       <c r="E48" s="33"/>
       <c r="F48" s="49" t="s">
@@ -3844,13 +4855,21 @@
       <c r="G48" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H48" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
-      <c r="B49" s="48"/>
-      <c r="C49" s="4"/>
+      <c r="B49" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>219</v>
+      </c>
       <c r="D49" s="33"/>
       <c r="E49" s="33"/>
       <c r="F49" s="49" t="s">
@@ -3859,128 +4878,182 @@
       <c r="G49" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H49" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
-      <c r="B50" s="48"/>
-      <c r="C50" s="4"/>
+      <c r="B50" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>224</v>
+      </c>
       <c r="D50" s="33"/>
       <c r="E50" s="33"/>
-      <c r="F50" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G50" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H50" s="3"/>
+      <c r="F50" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
-      <c r="B51" s="48"/>
-      <c r="C51" s="4"/>
+      <c r="B51" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>226</v>
+      </c>
       <c r="D51" s="33"/>
       <c r="E51" s="33"/>
-      <c r="F51" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G51" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H51" s="3"/>
+      <c r="F51" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
-      <c r="B52" s="48"/>
-      <c r="C52" s="4"/>
+      <c r="B52" s="35" t="s">
+        <v>229</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>228</v>
+      </c>
       <c r="D52" s="33"/>
       <c r="E52" s="33"/>
-      <c r="F52" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G52" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H52" s="3"/>
+      <c r="F52" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="I52" s="3"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
-      <c r="B53" s="48"/>
-      <c r="C53" s="4"/>
+      <c r="B53" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="D53" s="33"/>
       <c r="E53" s="33"/>
-      <c r="F53" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G53" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H53" s="3"/>
+      <c r="F53" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="I53" s="3"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
-      <c r="B54" s="48"/>
-      <c r="C54" s="4"/>
+      <c r="B54" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>232</v>
+      </c>
       <c r="D54" s="33"/>
       <c r="E54" s="33"/>
-      <c r="F54" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G54" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H54" s="3"/>
+      <c r="F54" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="I54" s="3"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
-      <c r="B55" s="48"/>
-      <c r="C55" s="4"/>
+      <c r="B55" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>234</v>
+      </c>
       <c r="D55" s="33"/>
       <c r="E55" s="33"/>
       <c r="F55" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="G55" s="52" t="s">
+      <c r="G55" s="10" t="s">
         <v>2</v>
       </c>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="4"/>
+      <c r="B56" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>236</v>
+      </c>
       <c r="D56" s="33"/>
       <c r="E56" s="33"/>
-      <c r="F56" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G56" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
+      <c r="F56" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="4"/>
+      <c r="B57" s="35" t="s">
+        <v>239</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>240</v>
+      </c>
       <c r="D57" s="33"/>
       <c r="E57" s="33"/>
       <c r="F57" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="G57" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
+      <c r="G57" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
@@ -4026,6 +5099,216 @@
       </c>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" s="48"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="33"/>
+      <c r="E61" s="33"/>
+      <c r="F61" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G61" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+      <c r="B62" s="48"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="33"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+      <c r="B63" s="48"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="33"/>
+      <c r="E63" s="33"/>
+      <c r="F63" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G63" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+      <c r="B64" s="48"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="33"/>
+      <c r="F64" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G64" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+      <c r="B65" s="48"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
+      <c r="F65" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G65" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="48"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="33"/>
+      <c r="E66" s="33"/>
+      <c r="F66" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" s="48"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="33"/>
+      <c r="F67" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G67" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+      <c r="B68" s="48"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="33"/>
+      <c r="E68" s="33"/>
+      <c r="F68" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G68" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+      <c r="B69" s="48"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="33"/>
+      <c r="E69" s="33"/>
+      <c r="F69" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G69" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+      <c r="B70" s="48"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="33"/>
+      <c r="E70" s="33"/>
+      <c r="F70" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G70" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+      <c r="B71" s="48"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="33"/>
+      <c r="E71" s="33"/>
+      <c r="F71" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G71" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+      <c r="B72" s="48"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="33"/>
+      <c r="E72" s="33"/>
+      <c r="F72" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G72" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+      <c r="B73" s="48"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="33"/>
+      <c r="E73" s="33"/>
+      <c r="F73" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G73" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+      <c r="B74" s="48"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="33"/>
+      <c r="E74" s="33"/>
+      <c r="F74" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="G74" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="D1:D11" xr:uid="{94F11FC0-660A-4BD3-84AA-75A655926AE4}"/>
@@ -4086,9 +5369,56 @@
     <hyperlink ref="G29" r:id="rId53" xr:uid="{5FCD94FB-830C-40AA-8545-58392F63DFE5}"/>
     <hyperlink ref="F30" r:id="rId54" xr:uid="{C2F2D5AA-04BD-4343-A515-6A214A792C57}"/>
     <hyperlink ref="G30" r:id="rId55" xr:uid="{1CF69C89-A2C7-4CCE-AEBC-798BA1CBD529}"/>
+    <hyperlink ref="G31" r:id="rId56" xr:uid="{3E841AD7-3D63-456C-B138-7B15EB2DCE69}"/>
+    <hyperlink ref="G32" r:id="rId57" xr:uid="{F255108A-CF7E-4108-8B34-38C05BBE5C1A}"/>
+    <hyperlink ref="F31" r:id="rId58" xr:uid="{49468D3E-DFB6-40F7-86FA-B8CD9C5023BF}"/>
+    <hyperlink ref="G33" r:id="rId59" xr:uid="{0017C344-1C95-43CA-A56A-99C4B32A2939}"/>
+    <hyperlink ref="G34" r:id="rId60" xr:uid="{1CAE06B2-F283-446B-9688-9A998EBC7101}"/>
+    <hyperlink ref="F33" r:id="rId61" xr:uid="{1763F2A1-9A81-48A1-82FE-A4FA4A8C5A63}"/>
+    <hyperlink ref="F34" r:id="rId62" xr:uid="{ED3FD7A8-6878-47EA-A0E2-A266941CC4FB}"/>
+    <hyperlink ref="G35" r:id="rId63" xr:uid="{874D2819-9677-4F72-9271-182014995B9F}"/>
+    <hyperlink ref="F35" r:id="rId64" xr:uid="{AB65F6F6-FD57-4075-A218-2110D77A186E}"/>
+    <hyperlink ref="G36" r:id="rId65" xr:uid="{B66F7BC2-AA92-43CF-997A-5E3B9B8AB15A}"/>
+    <hyperlink ref="F36" r:id="rId66" xr:uid="{7DB84370-5969-4BF5-B2A1-35117F9D493F}"/>
+    <hyperlink ref="G37" r:id="rId67" xr:uid="{51E7BF68-4A35-4973-8CB3-A3FBEAE2DBCD}"/>
+    <hyperlink ref="G38" r:id="rId68" xr:uid="{54FE68D3-0D9B-481E-815A-B2D27F335148}"/>
+    <hyperlink ref="F38" r:id="rId69" xr:uid="{795FCB86-691E-42B7-B147-AB958D988DE4}"/>
+    <hyperlink ref="F37" r:id="rId70" xr:uid="{27EFF91C-FF47-40AC-9743-AA680A7593AE}"/>
+    <hyperlink ref="G39" r:id="rId71" xr:uid="{5420420C-CF12-4CF5-9F48-F4918F7A5C1A}"/>
+    <hyperlink ref="F39" r:id="rId72" xr:uid="{7D6758A7-1BFA-4EF2-AE93-CEA864A3A86C}"/>
+    <hyperlink ref="G40" r:id="rId73" xr:uid="{69ADD537-C57E-4B4B-8EBE-92443353E177}"/>
+    <hyperlink ref="F40" r:id="rId74" xr:uid="{2852DD3B-12C0-4BD8-8AB0-ECE40197CCD5}"/>
+    <hyperlink ref="G41" r:id="rId75" location="d=gs_cit&amp;t=1698206552797&amp;u=%2Fscholar%3Fq%3Dinfo%3AjxH1Uk61gvoJ%3Ascholar.google.com%2F%26output%3Dcite%26scirp%3D0%26hl%3Den" xr:uid="{FE955CCB-8D56-4167-9F97-28154458F65E}"/>
+    <hyperlink ref="F41" r:id="rId76" xr:uid="{1EC12A37-FA01-4A9E-8A62-D12A74BB696E}"/>
+    <hyperlink ref="G42" r:id="rId77" xr:uid="{46309DC7-373B-49ED-8838-83DEC782CA7B}"/>
+    <hyperlink ref="F44" r:id="rId78" xr:uid="{75048957-1FD2-4801-8211-885239ABE194}"/>
+    <hyperlink ref="G44" r:id="rId79" xr:uid="{4ACA27BA-4015-42F9-9809-27A9CBAF8008}"/>
+    <hyperlink ref="G43" r:id="rId80" xr:uid="{3299C492-C48C-4DFD-B7D4-5E40046C7C3B}"/>
+    <hyperlink ref="F43" r:id="rId81" xr:uid="{A4206D4A-FBA3-4707-8177-554D19170C76}"/>
+    <hyperlink ref="G45" r:id="rId82" location="d=gs_cit&amp;t=1698208004725&amp;u=%2Fscholar%3Fq%3Dinfo%3ALrPNPdmMzoAJ%3Ascholar.google.com%2F%26output%3Dcite%26scirp%3D0%26hl%3Den" xr:uid="{BC660279-8D44-411F-9B60-D2C8484B4CD3}"/>
+    <hyperlink ref="F46" r:id="rId83" xr:uid="{F4B848A2-0234-4AC6-97FB-7C70F57FBD79}"/>
+    <hyperlink ref="G46" r:id="rId84" location="d=gs_cit&amp;t=1698208159901&amp;u=%2Fscholar%3Fq%3Dinfo%3At7em8QI0BvcJ%3Ascholar.google.com%2F%26output%3Dcite%26scirp%3D0%26hl%3Den" xr:uid="{427FAEB8-79DA-45B7-82CC-5353E212A3CF}"/>
+    <hyperlink ref="F45" r:id="rId85" xr:uid="{5DCC5679-B773-4E9D-B494-F6BFAF3CF225}"/>
+    <hyperlink ref="F32" r:id="rId86" xr:uid="{36BC04A3-D141-45A1-9CC2-02852953993F}"/>
+    <hyperlink ref="G47" r:id="rId87" location="d=gs_cit&amp;t=1698216765892&amp;u=%2Fscholar%3Fq%3Dinfo%3AXO81cDQ-kYsJ%3Ascholar.google.com%2F%26output%3Dcite%26scirp%3D0%26hl%3Den" xr:uid="{8E0C3060-50CF-4A8A-B8B3-555C3E56F3ED}"/>
+    <hyperlink ref="F47" r:id="rId88" xr:uid="{B53178AF-E931-4CB0-8C9D-D785707A124B}"/>
+    <hyperlink ref="G50" r:id="rId89" xr:uid="{EEEF8262-DC52-4D9B-A275-3C731E1214C8}"/>
+    <hyperlink ref="F50" r:id="rId90" xr:uid="{4DF4A13C-8805-4534-9464-81098ED8B409}"/>
+    <hyperlink ref="G51" r:id="rId91" xr:uid="{762E895C-0C83-4547-BD42-50F3837C3B96}"/>
+    <hyperlink ref="F51" r:id="rId92" xr:uid="{7D00E651-95AD-4DF8-B5D2-707DBA33745B}"/>
+    <hyperlink ref="G52" r:id="rId93" xr:uid="{CB9FE6CE-6A61-44A7-9A0A-7267A1B06382}"/>
+    <hyperlink ref="F52" r:id="rId94" xr:uid="{D20E8C9A-BF83-4C3E-8076-8065EE7FD87A}"/>
+    <hyperlink ref="G53" r:id="rId95" xr:uid="{00406BD4-55AE-4596-A31F-5250D90F3A99}"/>
+    <hyperlink ref="F53" r:id="rId96" xr:uid="{5A84B527-8648-4E3D-B6AD-1F5B98E0677B}"/>
+    <hyperlink ref="G54" r:id="rId97" xr:uid="{003F69EC-D924-476E-B02E-C20FA981A636}"/>
+    <hyperlink ref="F54" r:id="rId98" xr:uid="{93986BEB-46D1-4827-AC45-11054B555A61}"/>
+    <hyperlink ref="G55" r:id="rId99" xr:uid="{244D7282-126C-495A-ACF4-AD6FEDFEC481}"/>
+    <hyperlink ref="G56" r:id="rId100" xr:uid="{C3EFFC50-EAEF-4250-B1C5-6ECC117841E7}"/>
+    <hyperlink ref="F56" r:id="rId101" xr:uid="{6FD69EE7-DB38-4323-B56D-4EF3C7AC1FEC}"/>
+    <hyperlink ref="G57" r:id="rId102" xr:uid="{99B743B3-0085-4BB1-AC7D-07BF0833EB12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId56"/>
+  <pageSetup orientation="portrait" r:id="rId103"/>
 </worksheet>
 </file>
 
@@ -4096,8 +5426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3CB709-2DCD-458D-A9A0-63BE3420956F}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4106,15 +5436,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4233,4 +5563,114 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676FAC0A-2CA9-4FB7-B41D-06359F5CFD3D}">
+  <dimension ref="A2:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="75" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" s="75" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" s="76" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="70">
+        <v>1</v>
+      </c>
+      <c r="B3" s="66" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="66" t="s">
+        <v>206</v>
+      </c>
+      <c r="D3" s="67">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="E3" s="72">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="71">
+        <v>2</v>
+      </c>
+      <c r="B4" s="68" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4" s="68" t="s">
+        <v>208</v>
+      </c>
+      <c r="D4" s="69">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="E4" s="73">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="70">
+        <v>3</v>
+      </c>
+      <c r="B5" s="66" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="67">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="E5" s="72">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="77">
+        <v>4</v>
+      </c>
+      <c r="B6" s="78" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" s="78" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="79">
+        <v>0.77149999999999996</v>
+      </c>
+      <c r="E6" s="80">
+        <v>2015</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>